<commit_message>
Html Files for teams
Lots of stuff
</commit_message>
<xml_diff>
--- a/BBLTeams.xlsx
+++ b/BBLTeams.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="160">
   <si>
     <t>Adelaide Strikers</t>
   </si>
@@ -493,6 +493,12 @@
   </si>
   <si>
     <t>Nick Buchanan</t>
+  </si>
+  <si>
+    <t>Tom Andrews</t>
+  </si>
+  <si>
+    <t>Gurinder Sandu</t>
   </si>
 </sst>
 </file>
@@ -1335,8 +1341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1845,8 +1851,14 @@
       <c r="G20" t="s">
         <v>153</v>
       </c>
+      <c r="H20" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>158</v>
+      </c>
       <c r="G21" t="s">
         <v>154</v>
       </c>
@@ -1863,5 +1875,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>